<commit_message>
Bulk Upload Catalog Excel Updated
</commit_message>
<xml_diff>
--- a/src/assets/samples/CatalogProductUpload.xlsx
+++ b/src/assets/samples/CatalogProductUpload.xlsx
@@ -8,44 +8,80 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="data" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t xml:space="preserve">CatalogId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ProductId</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
+    <t xml:space="preserve">ParentCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IsFeatured</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IsShowOnHomePage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RetailPriceInclusive</t>
+  </si>
+  <si>
     <t xml:space="preserve">RetailPrice</t>
   </si>
   <si>
     <t xml:space="preserve">RetailShippingPrice</t>
   </si>
   <si>
-    <t xml:space="preserve">RetailPriceInclusive</t>
-  </si>
-  <si>
     <t xml:space="preserve">Discount</t>
   </si>
   <si>
     <t xml:space="preserve">DiscountType</t>
   </si>
   <si>
+    <t xml:space="preserve">FinalPrice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IsOutOfStock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ModelNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SellerId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CategoryId</t>
+  </si>
+  <si>
     <t xml:space="preserve">IsFeaturedProduct</t>
   </si>
   <si>
@@ -56,9 +92,6 @@
   </si>
   <si>
     <t xml:space="preserve">HomePageProductDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CatalogProductMappingIsActive</t>
   </si>
 </sst>
 </file>
@@ -70,8 +103,9 @@
   </numFmts>
   <fonts count="4">
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -155,18 +189,42 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X1" activeCellId="0" sqref="X1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="5.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="6.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="4.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="7.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="2.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="7.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="10.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="15.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="24.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="17.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="26.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="25" style="0" width="8.36"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -205,15 +263,48 @@
       </c>
       <c r="M1" s="0" t="s">
         <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>